<commit_message>
Update packet layout spreadsheet
</commit_message>
<xml_diff>
--- a/Tori.xlsx
+++ b/Tori.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin.Spinar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin.Spinar\Documents\Visual Studio 2015\Projects\tori\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="34">
   <si>
     <t>To Entry</t>
   </si>
@@ -512,7 +512,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,22 +826,22 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B11" s="7">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E11" s="7">
-        <v>8</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="7">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>14</v>
@@ -902,21 +902,21 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B13" s="7">
         <v>16</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E13" s="7">
         <v>16</v>
       </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13">
+      <c r="G13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="7">
         <v>16</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -940,22 +940,22 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B14" s="7">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E14" s="7">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="H14" s="7">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>19</v>
@@ -978,22 +978,22 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H15" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -1005,96 +1005,90 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H16" s="7">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="7">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="7">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="7">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>16</v>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="10">
+        <v>41</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="10">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="10">
-        <v>41</v>
-      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="10" t="s">
         <v>20</v>
@@ -1119,12 +1113,8 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="10">
-        <v>41</v>
-      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
       <c r="J21" s="6" t="s">
         <v>31</v>
       </c>
@@ -1133,14 +1123,6 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
       <c r="J22" s="16" t="s">
         <v>22</v>
       </c>

</xml_diff>